<commit_message>
Comentarios en las celdas del formato de participantes en Excel.
</commit_message>
<xml_diff>
--- a/docs/formatos/participantes.xlsx
+++ b/docs/formatos/participantes.xlsx
@@ -26,15 +26,224 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Link gerencial</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valor único. No. Carnet o el generado (puede ser alfa numérico)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valor único. Alfanumérico. Puede ser N.cédula, el correo, etc. OBLIGATORIO.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfabético. Sin punto. Sin comas. Se permite espacio, ñ, acentos.
+OBLIGATORIO.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfabético. Sin punto. Sin comas. Se permite espacio, ñ, acentos.
+OBLIGATORIO.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dd/mm/aaaa este será la fecha en que queda registrado el usuario en la plataforma. OJO: La celda debe estar formateada como Texto, no como fecha.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Puede ser alfanumérico. 
+OBLIGATORIO.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valor único para cada participante.
+OBLIGATORIO.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Numérico: 
+0 (no ve competencias).
+1 (si ve competencias).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>OBLIGATORIO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfanuméricos y puede venir vacío.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfanuméricos y puede venir vacío.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfanuméricos y puede venir vacío.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alfanuméricos y puede venir vacío.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Este campo se usará para el filtro de los programas. Si este campo viene vacío los usuarios ven todos los programas asignados a la empresa.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Código Empleado</t>
   </si>
   <si>
-    <t>Usuario / login</t>
-  </si>
-  <si>
     <t>Nombres</t>
   </si>
   <si>
@@ -50,15 +259,6 @@
     <t xml:space="preserve">Nivel </t>
   </si>
   <si>
-    <t>fecha de registo</t>
-  </si>
-  <si>
-    <t>contraseña</t>
-  </si>
-  <si>
-    <t>Correo Electrónico</t>
-  </si>
-  <si>
     <t>campo 1</t>
   </si>
   <si>
@@ -93,13 +293,25 @@
   </si>
   <si>
     <t>Nivel ejemplo</t>
+  </si>
+  <si>
+    <t>Fecha de registro</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t>Usuario / Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +353,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -476,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -505,43 +724,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="M1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="N1" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -549,35 +768,35 @@
         <v>1002</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,5 +884,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Select de niveles con usuarios asignados en el formulario del calendario. Ajustes en la carga masiva de participantes agregando la columna de activo.
</commit_message>
<xml_diff>
--- a/docs/formatos/participantes.xlsx
+++ b/docs/formatos/participantes.xlsx
@@ -234,12 +234,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="O2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Numérico: 
+0 (inactivo).
+1 (activo).</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Código Empleado</t>
   </si>
@@ -305,6 +321,9 @@
   </si>
   <si>
     <t>Usuario / Login</t>
+  </si>
+  <si>
+    <t>Activo</t>
   </si>
 </sst>
 </file>
@@ -696,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +738,7 @@
     <col min="14" max="14" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -762,8 +781,11 @@
       <c r="N1" s="10" t="s">
         <v>5</v>
       </c>
+      <c r="O1" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1002</v>
       </c>
@@ -798,8 +820,11 @@
       <c r="N2" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -807,7 +832,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -815,7 +840,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -831,7 +856,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -847,7 +872,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -863,7 +888,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>

</xml_diff>

<commit_message>
Correo obligatorio en el registro de usuarios
</commit_message>
<xml_diff>
--- a/docs/formatos/participantes.xlsx
+++ b/docs/formatos/participantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\formacion2.0\docs\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,7 +40,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor único. No. Carnet o el generado (puede ser alfa numérico)</t>
         </r>
@@ -54,7 +54,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor único. Alfanumérico. Puede ser N.cédula, el correo, etc. OBLIGATORIO.</t>
         </r>
@@ -68,7 +68,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfabético. Sin punto. Sin comas. Se permite espacio, ñ, acentos.
 OBLIGATORIO.</t>
@@ -83,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfabético. Sin punto. Sin comas. Se permite espacio, ñ, acentos.
 OBLIGATORIO.</t>
@@ -98,7 +98,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>dd/mm/aaaa este será la fecha en que queda registrado el usuario en la plataforma. OJO: La celda debe estar formateada como Texto, no como fecha.</t>
         </r>
@@ -112,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Puede ser alfanumérico. 
 OBLIGATORIO.</t>
@@ -127,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor único para cada participante.
 OBLIGATORIO.</t>
@@ -142,7 +142,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numérico: 
 0 (no ve competencias).
@@ -158,7 +158,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>OBLIGATORIO</t>
         </r>
@@ -172,7 +172,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfanuméricos y puede venir vacío.</t>
         </r>
@@ -186,7 +186,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfanuméricos y puede venir vacío.</t>
         </r>
@@ -200,7 +200,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfanuméricos y puede venir vacío.</t>
         </r>
@@ -214,7 +214,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alfanuméricos y puede venir vacío.</t>
         </r>
@@ -228,7 +228,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Este campo se usará para el filtro de los programas. Si este campo viene vacío los usuarios ven todos los programas asignados a la empresa.</t>
         </r>
@@ -242,7 +242,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numérico: 
 0 (inactivo).
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,7 +378,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>